<commit_message>
INS03 Segunda Aba P Média
</commit_message>
<xml_diff>
--- a/fontes/assets/reportINS03.xlsx
+++ b/fontes/assets/reportINS03.xlsx
@@ -7,7 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="INS03 VIP 22,5M" sheetId="1" r:id="rId4"/>
+    <sheet name="INS03 Prioridade Baixa" sheetId="1" r:id="rId4"/>
+    <sheet name="INS03 Prioridade Média" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="0"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Relatório de Chamados Atendidos dentro do TMS INS03 - Meta 95%</t>
   </si>
@@ -23,7 +24,7 @@
     <t>95% dos Chamados Atendidos</t>
   </si>
   <si>
-    <t>Total de Tickets Solucionados dentro SLA VIP 22,5M</t>
+    <t>Total de Tickets Solucionados Prioridade Baixa</t>
   </si>
   <si>
     <t>Total de Tickets Solucionados</t>
@@ -102,6 +103,12 @@
   </si>
   <si>
     <t>Sla Consumido</t>
+  </si>
+  <si>
+    <t>Sim/Não</t>
+  </si>
+  <si>
+    <t>Total de Tickets Solucionados Prioridade Média</t>
   </si>
 </sst>
 </file>
@@ -475,7 +482,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="80" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B6" sqref="B6"/>
@@ -507,29 +514,30 @@
     <col min="22" max="22" width="4.570313" bestFit="true" customWidth="true" style="4"/>
     <col min="23" max="23" width="24.708252" bestFit="true" customWidth="true" style="4"/>
     <col min="24" max="24" width="16.424561" bestFit="true" customWidth="true" style="4"/>
-    <col min="25" max="25" width="9.10" hidden="true" style="0"/>
+    <col min="25" max="25" width="16.424561" bestFit="true" customWidth="true" style="4"/>
+    <col min="26" max="26" width="9.283447" bestFit="true" customWidth="true" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <f>COUNTIF(Y9:Y9,"&lt;=1350")</f>
+        <f>COUNTIF(Z9:Z9,"=0")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:26">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -538,7 +546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -547,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:26">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -620,8 +628,191 @@
       <c r="X8" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Y8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="O9" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:Z9"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="80" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="62" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15" customWidth="true" style="0"/>
+    <col min="3" max="3" width="85" customWidth="true" style="0"/>
+    <col min="4" max="4" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="80" customWidth="true" style="0"/>
+    <col min="8" max="8" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="17.567139" bestFit="true" customWidth="true" style="4"/>
+    <col min="18" max="18" width="17.567139" bestFit="true" customWidth="true" style="4"/>
+    <col min="19" max="19" width="23.422852" bestFit="true" customWidth="true" style="4"/>
+    <col min="20" max="20" width="17.567139" bestFit="true" customWidth="true" style="4"/>
+    <col min="21" max="21" width="32.991943" bestFit="true" customWidth="true" style="4"/>
+    <col min="22" max="22" width="4.570313" bestFit="true" customWidth="true" style="4"/>
+    <col min="23" max="23" width="24.708252" bestFit="true" customWidth="true" style="4"/>
+    <col min="24" max="24" width="16.424561" bestFit="true" customWidth="true" style="4"/>
+    <col min="25" max="25" width="16.424561" bestFit="true" customWidth="true" style="4"/>
+    <col min="26" max="26" width="9.283447" bestFit="true" customWidth="true" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3">
+        <f>COUNTIF(Z9:Z9,"=0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f>COUNTIF(B9:B9,"&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f>IF(B4,B4/B5,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="O9" s="5"/>
     </row>
   </sheetData>

</xml_diff>